<commit_message>
second commit added 2 tests
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>standard_user</t>
-  </si>
-  <si>
-    <t>locked_out_user</t>
   </si>
   <si>
     <t>problem_user</t>
@@ -357,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -382,7 +379,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -390,7 +387,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -398,15 +395,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4th excel utils pkg added
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="correct log" sheetId="1" r:id="rId1"/>
+    <sheet name="incorrect log" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +38,9 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>locked_out_user</t>
   </si>
 </sst>
 </file>
@@ -356,8 +360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -402,4 +406,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>